<commit_message>
Added Multiprocessing Added CreditCurve Cleaned up redundant import modules
</commit_message>
<xml_diff>
--- a/PythonMarketAnalytics/Market/MarketData.xlsx
+++ b/PythonMarketAnalytics/Market/MarketData.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zongjie\source\repos\zongjieshen\PythonMarketAnalytics\PythonMarketAnalytics\Market\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zongjie\source\repos\zongjieshen\RatesMarket\PythonMarketAnalytics\Market\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD7FED37-6FCD-486A-BBEA-353DE7DB4A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9663F63A-E247-4DC6-BE33-AB0F8082E262}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="5415" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{DDD47C20-C930-4AC7-80D9-7FCAB22FD09D}"/>
+    <workbookView xWindow="-28920" yWindow="5415" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{DDD47C20-C930-4AC7-80D9-7FCAB22FD09D}"/>
   </bookViews>
   <sheets>
     <sheet name="YieldCurve" sheetId="1" r:id="rId1"/>
-    <sheet name="InflationCurve" sheetId="2" r:id="rId2"/>
-    <sheet name="IndexFixing" sheetId="3" r:id="rId3"/>
+    <sheet name="CreditCurve" sheetId="4" r:id="rId2"/>
+    <sheet name="InflationCurve" sheetId="2" r:id="rId3"/>
+    <sheet name="IndexFixing" sheetId="3" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">YieldCurve!$A$1:$Q$955</definedName>
   </definedNames>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="181029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,9 +29,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -40,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18679" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18786" uniqueCount="1071">
   <si>
     <t>Context</t>
   </si>
@@ -3222,6 +3221,39 @@
   </si>
   <si>
     <t>USCPI</t>
+  </si>
+  <si>
+    <t>CreditDefaultSwap</t>
+  </si>
+  <si>
+    <t>CDS1Y</t>
+  </si>
+  <si>
+    <t>CDS3Y</t>
+  </si>
+  <si>
+    <t>CDS5Y</t>
+  </si>
+  <si>
+    <t>CDS6Y</t>
+  </si>
+  <si>
+    <t>CDS8Y</t>
+  </si>
+  <si>
+    <t>CDS9Y</t>
+  </si>
+  <si>
+    <t>CDS12Y</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t+1b+9Y                  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">t+1b+12y                  </t>
+  </si>
+  <si>
+    <t>RecoveryRate</t>
   </si>
 </sst>
 </file>
@@ -3231,7 +3263,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="#,##0_ ;[Red]\-#,##0\ "/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3332,6 +3364,12 @@
       <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -3891,7 +3929,7 @@
   <dimension ref="A1:Q955"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A956" sqref="A956"/>
+      <selection activeCell="F469" sqref="F469"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4074,7 +4112,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" hidden="1">
       <c r="A4" s="3" t="s">
         <v>17</v>
       </c>
@@ -4127,7 +4165,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" hidden="1">
       <c r="A5" s="3" t="s">
         <v>17</v>
       </c>
@@ -4286,7 +4324,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" hidden="1">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
@@ -4551,7 +4589,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" hidden="1">
       <c r="A13" s="3" t="s">
         <v>17</v>
       </c>
@@ -4604,7 +4642,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" hidden="1">
       <c r="A14" s="3" t="s">
         <v>17</v>
       </c>
@@ -4816,7 +4854,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:17">
+    <row r="18" spans="1:17" hidden="1">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -4975,7 +5013,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="21" spans="1:17">
+    <row r="21" spans="1:17" hidden="1">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
@@ -5028,7 +5066,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" hidden="1">
       <c r="A22" s="3" t="s">
         <v>17</v>
       </c>
@@ -5293,7 +5331,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:17">
+    <row r="27" spans="1:17" hidden="1">
       <c r="A27" s="3" t="s">
         <v>17</v>
       </c>
@@ -5346,7 +5384,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:17">
+    <row r="28" spans="1:17" hidden="1">
       <c r="A28" s="3" t="s">
         <v>17</v>
       </c>
@@ -6088,7 +6126,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="42" spans="1:17">
+    <row r="42" spans="1:17" hidden="1">
       <c r="A42" s="3" t="s">
         <v>17</v>
       </c>
@@ -6247,7 +6285,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:17">
+    <row r="45" spans="1:17" hidden="1">
       <c r="A45" s="3" t="s">
         <v>17</v>
       </c>
@@ -6300,7 +6338,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:17">
+    <row r="46" spans="1:17" hidden="1">
       <c r="A46" s="3" t="s">
         <v>17</v>
       </c>
@@ -6512,7 +6550,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="50" spans="1:17">
+    <row r="50" spans="1:17" hidden="1">
       <c r="A50" s="3" t="s">
         <v>17</v>
       </c>
@@ -6671,7 +6709,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="53" spans="1:17">
+    <row r="53" spans="1:17" hidden="1">
       <c r="A53" s="3" t="s">
         <v>17</v>
       </c>
@@ -6777,7 +6815,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:17">
+    <row r="55" spans="1:17" hidden="1">
       <c r="A55" s="3" t="s">
         <v>17</v>
       </c>
@@ -28234,7 +28272,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="460" spans="1:17" hidden="1">
+    <row r="460" spans="1:17">
       <c r="A460" s="3" t="s">
         <v>17</v>
       </c>
@@ -28285,7 +28323,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="461" spans="1:17" hidden="1">
+    <row r="461" spans="1:17">
       <c r="A461" s="3" t="s">
         <v>17</v>
       </c>
@@ -28336,7 +28374,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="462" spans="1:17" hidden="1">
+    <row r="462" spans="1:17">
       <c r="A462" s="3" t="s">
         <v>17</v>
       </c>
@@ -28387,7 +28425,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="463" spans="1:17" hidden="1">
+    <row r="463" spans="1:17">
       <c r="A463" s="3" t="s">
         <v>17</v>
       </c>
@@ -28438,7 +28476,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="464" spans="1:17" hidden="1">
+    <row r="464" spans="1:17">
       <c r="A464" s="3" t="s">
         <v>17</v>
       </c>
@@ -28489,7 +28527,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="465" spans="1:17" hidden="1">
+    <row r="465" spans="1:17">
       <c r="A465" s="3" t="s">
         <v>17</v>
       </c>
@@ -28540,7 +28578,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="466" spans="1:17" hidden="1">
+    <row r="466" spans="1:17">
       <c r="A466" s="3" t="s">
         <v>17</v>
       </c>
@@ -28591,7 +28629,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="467" spans="1:17" hidden="1">
+    <row r="467" spans="1:17">
       <c r="A467" s="3" t="s">
         <v>17</v>
       </c>
@@ -28642,7 +28680,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="468" spans="1:17" hidden="1">
+    <row r="468" spans="1:17">
       <c r="A468" s="3" t="s">
         <v>17</v>
       </c>
@@ -28693,7 +28731,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="469" spans="1:17" hidden="1">
+    <row r="469" spans="1:17">
       <c r="A469" s="3" t="s">
         <v>17</v>
       </c>
@@ -28744,7 +28782,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="470" spans="1:17" hidden="1">
+    <row r="470" spans="1:17">
       <c r="A470" s="3" t="s">
         <v>17</v>
       </c>
@@ -28795,7 +28833,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="471" spans="1:17" hidden="1">
+    <row r="471" spans="1:17">
       <c r="A471" s="3" t="s">
         <v>17</v>
       </c>
@@ -28846,7 +28884,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="472" spans="1:17" hidden="1">
+    <row r="472" spans="1:17">
       <c r="A472" s="3" t="s">
         <v>17</v>
       </c>
@@ -28897,7 +28935,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="473" spans="1:17" hidden="1">
+    <row r="473" spans="1:17">
       <c r="A473" s="3" t="s">
         <v>17</v>
       </c>
@@ -28948,7 +28986,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="474" spans="1:17" hidden="1">
+    <row r="474" spans="1:17">
       <c r="A474" s="3" t="s">
         <v>17</v>
       </c>
@@ -28999,7 +29037,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="475" spans="1:17" hidden="1">
+    <row r="475" spans="1:17">
       <c r="A475" s="3" t="s">
         <v>17</v>
       </c>
@@ -29050,7 +29088,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="476" spans="1:17" hidden="1">
+    <row r="476" spans="1:17">
       <c r="A476" s="3" t="s">
         <v>17</v>
       </c>
@@ -29101,7 +29139,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="477" spans="1:17" hidden="1">
+    <row r="477" spans="1:17">
       <c r="A477" s="3" t="s">
         <v>17</v>
       </c>
@@ -29152,7 +29190,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="478" spans="1:17" hidden="1">
+    <row r="478" spans="1:17">
       <c r="A478" s="3" t="s">
         <v>17</v>
       </c>
@@ -29203,7 +29241,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="479" spans="1:17" hidden="1">
+    <row r="479" spans="1:17">
       <c r="A479" s="3" t="s">
         <v>17</v>
       </c>
@@ -29254,7 +29292,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="480" spans="1:17" hidden="1">
+    <row r="480" spans="1:17">
       <c r="A480" s="3" t="s">
         <v>17</v>
       </c>
@@ -29305,7 +29343,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="481" spans="1:17" hidden="1">
+    <row r="481" spans="1:17">
       <c r="A481" s="3" t="s">
         <v>17</v>
       </c>
@@ -29356,7 +29394,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="482" spans="1:17" hidden="1">
+    <row r="482" spans="1:17">
       <c r="A482" s="3" t="s">
         <v>17</v>
       </c>
@@ -29407,7 +29445,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="483" spans="1:17" hidden="1">
+    <row r="483" spans="1:17">
       <c r="A483" s="3" t="s">
         <v>17</v>
       </c>
@@ -29458,7 +29496,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="484" spans="1:17" hidden="1">
+    <row r="484" spans="1:17">
       <c r="A484" s="3" t="s">
         <v>17</v>
       </c>
@@ -29509,7 +29547,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="485" spans="1:17" hidden="1">
+    <row r="485" spans="1:17">
       <c r="A485" s="3" t="s">
         <v>17</v>
       </c>
@@ -29560,7 +29598,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="486" spans="1:17" hidden="1">
+    <row r="486" spans="1:17">
       <c r="A486" s="3" t="s">
         <v>17</v>
       </c>
@@ -29611,7 +29649,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="487" spans="1:17" hidden="1">
+    <row r="487" spans="1:17">
       <c r="A487" s="3" t="s">
         <v>17</v>
       </c>
@@ -29662,7 +29700,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="488" spans="1:17" hidden="1">
+    <row r="488" spans="1:17">
       <c r="A488" s="3" t="s">
         <v>17</v>
       </c>
@@ -29713,7 +29751,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="489" spans="1:17" hidden="1">
+    <row r="489" spans="1:17">
       <c r="A489" s="3" t="s">
         <v>17</v>
       </c>
@@ -29764,7 +29802,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="490" spans="1:17" hidden="1">
+    <row r="490" spans="1:17">
       <c r="A490" s="3" t="s">
         <v>17</v>
       </c>
@@ -29815,7 +29853,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="491" spans="1:17" hidden="1">
+    <row r="491" spans="1:17">
       <c r="A491" s="3" t="s">
         <v>17</v>
       </c>
@@ -29866,7 +29904,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="492" spans="1:17" hidden="1">
+    <row r="492" spans="1:17">
       <c r="A492" s="3" t="s">
         <v>17</v>
       </c>
@@ -29917,7 +29955,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="493" spans="1:17" hidden="1">
+    <row r="493" spans="1:17">
       <c r="A493" s="3" t="s">
         <v>17</v>
       </c>
@@ -29968,7 +30006,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="494" spans="1:17" hidden="1">
+    <row r="494" spans="1:17">
       <c r="A494" s="3" t="s">
         <v>17</v>
       </c>
@@ -30019,7 +30057,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="495" spans="1:17" hidden="1">
+    <row r="495" spans="1:17">
       <c r="A495" s="3" t="s">
         <v>17</v>
       </c>
@@ -30070,7 +30108,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="496" spans="1:17" hidden="1">
+    <row r="496" spans="1:17">
       <c r="A496" s="3" t="s">
         <v>17</v>
       </c>
@@ -30121,7 +30159,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="497" spans="1:17" hidden="1">
+    <row r="497" spans="1:17">
       <c r="A497" s="3" t="s">
         <v>17</v>
       </c>
@@ -30172,7 +30210,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="498" spans="1:17" hidden="1">
+    <row r="498" spans="1:17">
       <c r="A498" s="3" t="s">
         <v>17</v>
       </c>
@@ -30223,7 +30261,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="499" spans="1:17" hidden="1">
+    <row r="499" spans="1:17">
       <c r="A499" s="3" t="s">
         <v>17</v>
       </c>
@@ -30274,7 +30312,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="500" spans="1:17" hidden="1">
+    <row r="500" spans="1:17">
       <c r="A500" s="3" t="s">
         <v>17</v>
       </c>
@@ -30325,7 +30363,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="501" spans="1:17" hidden="1">
+    <row r="501" spans="1:17">
       <c r="A501" s="3" t="s">
         <v>17</v>
       </c>
@@ -30376,7 +30414,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="502" spans="1:17" hidden="1">
+    <row r="502" spans="1:17">
       <c r="A502" s="3" t="s">
         <v>17</v>
       </c>
@@ -30427,7 +30465,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="503" spans="1:17" hidden="1">
+    <row r="503" spans="1:17">
       <c r="A503" s="3" t="s">
         <v>17</v>
       </c>
@@ -30478,7 +30516,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="504" spans="1:17" hidden="1">
+    <row r="504" spans="1:17">
       <c r="A504" s="3" t="s">
         <v>17</v>
       </c>
@@ -30529,7 +30567,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="505" spans="1:17" hidden="1">
+    <row r="505" spans="1:17">
       <c r="A505" s="3" t="s">
         <v>17</v>
       </c>
@@ -30580,7 +30618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="506" spans="1:17" hidden="1">
+    <row r="506" spans="1:17">
       <c r="A506" s="3" t="s">
         <v>17</v>
       </c>
@@ -30631,7 +30669,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="507" spans="1:17" hidden="1">
+    <row r="507" spans="1:17">
       <c r="A507" s="3" t="s">
         <v>17</v>
       </c>
@@ -30682,7 +30720,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="508" spans="1:17" hidden="1">
+    <row r="508" spans="1:17">
       <c r="A508" s="3" t="s">
         <v>17</v>
       </c>
@@ -30733,7 +30771,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="509" spans="1:17" hidden="1">
+    <row r="509" spans="1:17">
       <c r="A509" s="3" t="s">
         <v>17</v>
       </c>
@@ -30784,7 +30822,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="510" spans="1:17" hidden="1">
+    <row r="510" spans="1:17">
       <c r="A510" s="3" t="s">
         <v>17</v>
       </c>
@@ -30835,7 +30873,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="511" spans="1:17" hidden="1">
+    <row r="511" spans="1:17">
       <c r="A511" s="3" t="s">
         <v>17</v>
       </c>
@@ -30886,7 +30924,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="512" spans="1:17" hidden="1">
+    <row r="512" spans="1:17">
       <c r="A512" s="3" t="s">
         <v>17</v>
       </c>
@@ -30937,7 +30975,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="513" spans="1:17" hidden="1">
+    <row r="513" spans="1:17">
       <c r="A513" s="3" t="s">
         <v>17</v>
       </c>
@@ -30988,7 +31026,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="514" spans="1:17" hidden="1">
+    <row r="514" spans="1:17">
       <c r="A514" s="3" t="s">
         <v>17</v>
       </c>
@@ -31039,7 +31077,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="515" spans="1:17" hidden="1">
+    <row r="515" spans="1:17">
       <c r="A515" s="3" t="s">
         <v>17</v>
       </c>
@@ -31090,7 +31128,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="516" spans="1:17" hidden="1">
+    <row r="516" spans="1:17">
       <c r="A516" s="3" t="s">
         <v>17</v>
       </c>
@@ -31141,7 +31179,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="517" spans="1:17" hidden="1">
+    <row r="517" spans="1:17">
       <c r="A517" s="3" t="s">
         <v>17</v>
       </c>
@@ -31192,7 +31230,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="518" spans="1:17" hidden="1">
+    <row r="518" spans="1:17">
       <c r="A518" s="3" t="s">
         <v>17</v>
       </c>
@@ -31243,7 +31281,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="519" spans="1:17" hidden="1">
+    <row r="519" spans="1:17">
       <c r="A519" s="3" t="s">
         <v>17</v>
       </c>
@@ -31294,7 +31332,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="520" spans="1:17" hidden="1">
+    <row r="520" spans="1:17">
       <c r="A520" s="3" t="s">
         <v>17</v>
       </c>
@@ -31345,7 +31383,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="521" spans="1:17" hidden="1">
+    <row r="521" spans="1:17">
       <c r="A521" s="3" t="s">
         <v>17</v>
       </c>
@@ -31396,7 +31434,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="522" spans="1:17" hidden="1">
+    <row r="522" spans="1:17">
       <c r="A522" s="3" t="s">
         <v>17</v>
       </c>
@@ -31447,7 +31485,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="523" spans="1:17" hidden="1">
+    <row r="523" spans="1:17">
       <c r="A523" s="3" t="s">
         <v>17</v>
       </c>
@@ -31498,7 +31536,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="524" spans="1:17" hidden="1">
+    <row r="524" spans="1:17">
       <c r="A524" s="3" t="s">
         <v>17</v>
       </c>
@@ -31549,7 +31587,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="525" spans="1:17" hidden="1">
+    <row r="525" spans="1:17">
       <c r="A525" s="3" t="s">
         <v>17</v>
       </c>
@@ -31600,7 +31638,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="526" spans="1:17" hidden="1">
+    <row r="526" spans="1:17">
       <c r="A526" s="3" t="s">
         <v>17</v>
       </c>
@@ -31651,7 +31689,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="527" spans="1:17" hidden="1">
+    <row r="527" spans="1:17">
       <c r="A527" s="3" t="s">
         <v>17</v>
       </c>
@@ -31702,7 +31740,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="528" spans="1:17" hidden="1">
+    <row r="528" spans="1:17">
       <c r="A528" s="3" t="s">
         <v>17</v>
       </c>
@@ -31753,7 +31791,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="529" spans="1:17" hidden="1">
+    <row r="529" spans="1:17">
       <c r="A529" s="3" t="s">
         <v>17</v>
       </c>
@@ -31804,7 +31842,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="530" spans="1:17" hidden="1">
+    <row r="530" spans="1:17">
       <c r="A530" s="3" t="s">
         <v>17</v>
       </c>
@@ -31855,7 +31893,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="531" spans="1:17" hidden="1">
+    <row r="531" spans="1:17">
       <c r="A531" s="3" t="s">
         <v>17</v>
       </c>
@@ -31906,7 +31944,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="532" spans="1:17" hidden="1">
+    <row r="532" spans="1:17">
       <c r="A532" s="3" t="s">
         <v>17</v>
       </c>
@@ -31957,7 +31995,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="533" spans="1:17" hidden="1">
+    <row r="533" spans="1:17">
       <c r="A533" s="3" t="s">
         <v>17</v>
       </c>
@@ -32008,7 +32046,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="534" spans="1:17" hidden="1">
+    <row r="534" spans="1:17">
       <c r="A534" s="3" t="s">
         <v>17</v>
       </c>
@@ -32059,7 +32097,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="535" spans="1:17" hidden="1">
+    <row r="535" spans="1:17">
       <c r="A535" s="3" t="s">
         <v>17</v>
       </c>
@@ -32110,7 +32148,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="536" spans="1:17" hidden="1">
+    <row r="536" spans="1:17">
       <c r="A536" s="3" t="s">
         <v>17</v>
       </c>
@@ -32161,7 +32199,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="537" spans="1:17" hidden="1">
+    <row r="537" spans="1:17">
       <c r="A537" s="3" t="s">
         <v>17</v>
       </c>
@@ -32212,7 +32250,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="538" spans="1:17" hidden="1">
+    <row r="538" spans="1:17">
       <c r="A538" s="3" t="s">
         <v>17</v>
       </c>
@@ -32263,7 +32301,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="539" spans="1:17" hidden="1">
+    <row r="539" spans="1:17">
       <c r="A539" s="3" t="s">
         <v>17</v>
       </c>
@@ -32314,7 +32352,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="540" spans="1:17" hidden="1">
+    <row r="540" spans="1:17">
       <c r="A540" s="3" t="s">
         <v>17</v>
       </c>
@@ -32365,7 +32403,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="541" spans="1:17" hidden="1">
+    <row r="541" spans="1:17">
       <c r="A541" s="3" t="s">
         <v>17</v>
       </c>
@@ -32416,7 +32454,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="542" spans="1:17" hidden="1">
+    <row r="542" spans="1:17">
       <c r="A542" s="3" t="s">
         <v>17</v>
       </c>
@@ -32467,7 +32505,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="543" spans="1:17" hidden="1">
+    <row r="543" spans="1:17">
       <c r="A543" s="3" t="s">
         <v>17</v>
       </c>
@@ -32518,7 +32556,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="544" spans="1:17" hidden="1">
+    <row r="544" spans="1:17">
       <c r="A544" s="3" t="s">
         <v>17</v>
       </c>
@@ -32569,7 +32607,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="545" spans="1:17" hidden="1">
+    <row r="545" spans="1:17">
       <c r="A545" s="3" t="s">
         <v>17</v>
       </c>
@@ -32620,7 +32658,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="546" spans="1:17" hidden="1">
+    <row r="546" spans="1:17">
       <c r="A546" s="3" t="s">
         <v>17</v>
       </c>
@@ -32671,7 +32709,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="547" spans="1:17" hidden="1">
+    <row r="547" spans="1:17">
       <c r="A547" s="3" t="s">
         <v>17</v>
       </c>
@@ -32722,7 +32760,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="548" spans="1:17" hidden="1">
+    <row r="548" spans="1:17">
       <c r="A548" s="3" t="s">
         <v>17</v>
       </c>
@@ -32773,7 +32811,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="549" spans="1:17" hidden="1">
+    <row r="549" spans="1:17">
       <c r="A549" s="3" t="s">
         <v>17</v>
       </c>
@@ -32824,7 +32862,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="550" spans="1:17" hidden="1">
+    <row r="550" spans="1:17">
       <c r="A550" s="3" t="s">
         <v>17</v>
       </c>
@@ -32875,7 +32913,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="551" spans="1:17" hidden="1">
+    <row r="551" spans="1:17">
       <c r="A551" s="3" t="s">
         <v>17</v>
       </c>
@@ -32926,7 +32964,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="552" spans="1:17" hidden="1">
+    <row r="552" spans="1:17">
       <c r="A552" s="3" t="s">
         <v>17</v>
       </c>
@@ -32977,7 +33015,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="553" spans="1:17" hidden="1">
+    <row r="553" spans="1:17">
       <c r="A553" s="3" t="s">
         <v>17</v>
       </c>
@@ -33028,7 +33066,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="554" spans="1:17" hidden="1">
+    <row r="554" spans="1:17">
       <c r="A554" s="3" t="s">
         <v>17</v>
       </c>
@@ -33079,7 +33117,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="555" spans="1:17" hidden="1">
+    <row r="555" spans="1:17">
       <c r="A555" s="3" t="s">
         <v>17</v>
       </c>
@@ -33130,7 +33168,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="556" spans="1:17" hidden="1">
+    <row r="556" spans="1:17">
       <c r="A556" s="3" t="s">
         <v>17</v>
       </c>
@@ -33181,7 +33219,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="557" spans="1:17" hidden="1">
+    <row r="557" spans="1:17">
       <c r="A557" s="3" t="s">
         <v>17</v>
       </c>
@@ -33232,7 +33270,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="558" spans="1:17" hidden="1">
+    <row r="558" spans="1:17">
       <c r="A558" s="3" t="s">
         <v>17</v>
       </c>
@@ -33283,7 +33321,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="559" spans="1:17" hidden="1">
+    <row r="559" spans="1:17">
       <c r="A559" s="3" t="s">
         <v>17</v>
       </c>
@@ -33334,7 +33372,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="560" spans="1:17" hidden="1">
+    <row r="560" spans="1:17">
       <c r="A560" s="3" t="s">
         <v>17</v>
       </c>
@@ -33385,7 +33423,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="561" spans="1:17" hidden="1">
+    <row r="561" spans="1:17">
       <c r="A561" s="3" t="s">
         <v>17</v>
       </c>
@@ -33436,7 +33474,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="562" spans="1:17" hidden="1">
+    <row r="562" spans="1:17">
       <c r="A562" s="3" t="s">
         <v>17</v>
       </c>
@@ -33487,7 +33525,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="563" spans="1:17" hidden="1">
+    <row r="563" spans="1:17">
       <c r="A563" s="3" t="s">
         <v>17</v>
       </c>
@@ -33538,7 +33576,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="564" spans="1:17" hidden="1">
+    <row r="564" spans="1:17">
       <c r="A564" s="3" t="s">
         <v>17</v>
       </c>
@@ -33589,7 +33627,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="565" spans="1:17" hidden="1">
+    <row r="565" spans="1:17">
       <c r="A565" s="3" t="s">
         <v>17</v>
       </c>
@@ -33640,7 +33678,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="566" spans="1:17" hidden="1">
+    <row r="566" spans="1:17">
       <c r="A566" s="3" t="s">
         <v>17</v>
       </c>
@@ -33691,7 +33729,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="567" spans="1:17" hidden="1">
+    <row r="567" spans="1:17">
       <c r="A567" s="3" t="s">
         <v>17</v>
       </c>
@@ -33742,7 +33780,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="568" spans="1:17" hidden="1">
+    <row r="568" spans="1:17">
       <c r="A568" s="3" t="s">
         <v>17</v>
       </c>
@@ -33793,7 +33831,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="569" spans="1:17" hidden="1">
+    <row r="569" spans="1:17">
       <c r="A569" s="3" t="s">
         <v>17</v>
       </c>
@@ -33844,7 +33882,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="570" spans="1:17" hidden="1">
+    <row r="570" spans="1:17">
       <c r="A570" s="3" t="s">
         <v>17</v>
       </c>
@@ -33895,7 +33933,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="571" spans="1:17" hidden="1">
+    <row r="571" spans="1:17">
       <c r="A571" s="3" t="s">
         <v>17</v>
       </c>
@@ -33946,7 +33984,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="572" spans="1:17" hidden="1">
+    <row r="572" spans="1:17">
       <c r="A572" s="3" t="s">
         <v>17</v>
       </c>
@@ -33997,7 +34035,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="573" spans="1:17" hidden="1">
+    <row r="573" spans="1:17">
       <c r="A573" s="3" t="s">
         <v>17</v>
       </c>
@@ -34048,7 +34086,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="574" spans="1:17" hidden="1">
+    <row r="574" spans="1:17">
       <c r="A574" s="3" t="s">
         <v>17</v>
       </c>
@@ -34099,7 +34137,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="575" spans="1:17" hidden="1">
+    <row r="575" spans="1:17">
       <c r="A575" s="3" t="s">
         <v>17</v>
       </c>
@@ -34150,7 +34188,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="576" spans="1:17" hidden="1">
+    <row r="576" spans="1:17">
       <c r="A576" s="3" t="s">
         <v>17</v>
       </c>
@@ -34201,7 +34239,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="577" spans="1:17" hidden="1">
+    <row r="577" spans="1:17">
       <c r="A577" s="3" t="s">
         <v>17</v>
       </c>
@@ -34252,7 +34290,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="578" spans="1:17" hidden="1">
+    <row r="578" spans="1:17">
       <c r="A578" s="3" t="s">
         <v>17</v>
       </c>
@@ -34303,7 +34341,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="579" spans="1:17" hidden="1">
+    <row r="579" spans="1:17">
       <c r="A579" s="3" t="s">
         <v>17</v>
       </c>
@@ -34354,7 +34392,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="580" spans="1:17" hidden="1">
+    <row r="580" spans="1:17">
       <c r="A580" s="3" t="s">
         <v>17</v>
       </c>
@@ -34405,7 +34443,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="581" spans="1:17" hidden="1">
+    <row r="581" spans="1:17">
       <c r="A581" s="3" t="s">
         <v>17</v>
       </c>
@@ -34456,7 +34494,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="582" spans="1:17" hidden="1">
+    <row r="582" spans="1:17">
       <c r="A582" s="3" t="s">
         <v>17</v>
       </c>
@@ -34507,7 +34545,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="583" spans="1:17" hidden="1">
+    <row r="583" spans="1:17">
       <c r="A583" s="3" t="s">
         <v>17</v>
       </c>
@@ -34558,7 +34596,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="584" spans="1:17" hidden="1">
+    <row r="584" spans="1:17">
       <c r="A584" s="3" t="s">
         <v>17</v>
       </c>
@@ -34609,7 +34647,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="585" spans="1:17" hidden="1">
+    <row r="585" spans="1:17">
       <c r="A585" s="3" t="s">
         <v>17</v>
       </c>
@@ -34660,7 +34698,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="586" spans="1:17" hidden="1">
+    <row r="586" spans="1:17">
       <c r="A586" s="3" t="s">
         <v>17</v>
       </c>
@@ -34711,7 +34749,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="587" spans="1:17" hidden="1">
+    <row r="587" spans="1:17">
       <c r="A587" s="3" t="s">
         <v>17</v>
       </c>
@@ -34762,7 +34800,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="588" spans="1:17" hidden="1">
+    <row r="588" spans="1:17">
       <c r="A588" s="3" t="s">
         <v>17</v>
       </c>
@@ -34813,7 +34851,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="589" spans="1:17" hidden="1">
+    <row r="589" spans="1:17">
       <c r="A589" s="3" t="s">
         <v>17</v>
       </c>
@@ -34864,7 +34902,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="590" spans="1:17" hidden="1">
+    <row r="590" spans="1:17">
       <c r="A590" s="3" t="s">
         <v>17</v>
       </c>
@@ -34915,7 +34953,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="591" spans="1:17" hidden="1">
+    <row r="591" spans="1:17">
       <c r="A591" s="3" t="s">
         <v>17</v>
       </c>
@@ -34966,7 +35004,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="592" spans="1:17" hidden="1">
+    <row r="592" spans="1:17">
       <c r="A592" s="3" t="s">
         <v>17</v>
       </c>
@@ -35017,7 +35055,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="593" spans="1:17" hidden="1">
+    <row r="593" spans="1:17">
       <c r="A593" s="3" t="s">
         <v>17</v>
       </c>
@@ -35068,7 +35106,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="594" spans="1:17" hidden="1">
+    <row r="594" spans="1:17">
       <c r="A594" s="3" t="s">
         <v>17</v>
       </c>
@@ -35119,7 +35157,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="595" spans="1:17" hidden="1">
+    <row r="595" spans="1:17">
       <c r="A595" s="3" t="s">
         <v>17</v>
       </c>
@@ -35170,7 +35208,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="596" spans="1:17" hidden="1">
+    <row r="596" spans="1:17">
       <c r="A596" s="3" t="s">
         <v>17</v>
       </c>
@@ -35221,7 +35259,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="597" spans="1:17" hidden="1">
+    <row r="597" spans="1:17">
       <c r="A597" s="3" t="s">
         <v>17</v>
       </c>
@@ -35272,7 +35310,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="598" spans="1:17" hidden="1">
+    <row r="598" spans="1:17">
       <c r="A598" s="3" t="s">
         <v>17</v>
       </c>
@@ -35323,7 +35361,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="599" spans="1:17" hidden="1">
+    <row r="599" spans="1:17">
       <c r="A599" s="3" t="s">
         <v>17</v>
       </c>
@@ -35374,7 +35412,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="600" spans="1:17" hidden="1">
+    <row r="600" spans="1:17">
       <c r="A600" s="3" t="s">
         <v>17</v>
       </c>
@@ -35425,7 +35463,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="601" spans="1:17" hidden="1">
+    <row r="601" spans="1:17">
       <c r="A601" s="3" t="s">
         <v>17</v>
       </c>
@@ -35476,7 +35514,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="602" spans="1:17" hidden="1">
+    <row r="602" spans="1:17">
       <c r="A602" s="3" t="s">
         <v>17</v>
       </c>
@@ -35527,7 +35565,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="603" spans="1:17" hidden="1">
+    <row r="603" spans="1:17">
       <c r="A603" s="3" t="s">
         <v>17</v>
       </c>
@@ -35578,7 +35616,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="604" spans="1:17" hidden="1">
+    <row r="604" spans="1:17">
       <c r="A604" s="3" t="s">
         <v>17</v>
       </c>
@@ -35629,7 +35667,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="605" spans="1:17" hidden="1">
+    <row r="605" spans="1:17">
       <c r="A605" s="3" t="s">
         <v>17</v>
       </c>
@@ -35680,7 +35718,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="606" spans="1:17" hidden="1">
+    <row r="606" spans="1:17">
       <c r="A606" s="3" t="s">
         <v>17</v>
       </c>
@@ -35731,7 +35769,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="607" spans="1:17" hidden="1">
+    <row r="607" spans="1:17">
       <c r="A607" s="3" t="s">
         <v>17</v>
       </c>
@@ -35782,7 +35820,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="608" spans="1:17" hidden="1">
+    <row r="608" spans="1:17">
       <c r="A608" s="3" t="s">
         <v>17</v>
       </c>
@@ -35833,7 +35871,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="609" spans="1:17" hidden="1">
+    <row r="609" spans="1:17">
       <c r="A609" s="3" t="s">
         <v>17</v>
       </c>
@@ -35884,7 +35922,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="610" spans="1:17" hidden="1">
+    <row r="610" spans="1:17">
       <c r="A610" s="3" t="s">
         <v>17</v>
       </c>
@@ -35935,7 +35973,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="611" spans="1:17" hidden="1">
+    <row r="611" spans="1:17">
       <c r="A611" s="3" t="s">
         <v>17</v>
       </c>
@@ -35986,7 +36024,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="612" spans="1:17" hidden="1">
+    <row r="612" spans="1:17">
       <c r="A612" s="3" t="s">
         <v>17</v>
       </c>
@@ -36037,7 +36075,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="613" spans="1:17" hidden="1">
+    <row r="613" spans="1:17">
       <c r="A613" s="3" t="s">
         <v>17</v>
       </c>
@@ -36088,7 +36126,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="614" spans="1:17" hidden="1">
+    <row r="614" spans="1:17">
       <c r="A614" s="3" t="s">
         <v>17</v>
       </c>
@@ -36139,7 +36177,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="615" spans="1:17" hidden="1">
+    <row r="615" spans="1:17">
       <c r="A615" s="3" t="s">
         <v>17</v>
       </c>
@@ -36190,7 +36228,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="616" spans="1:17" hidden="1">
+    <row r="616" spans="1:17">
       <c r="A616" s="3" t="s">
         <v>17</v>
       </c>
@@ -36241,7 +36279,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="617" spans="1:17" hidden="1">
+    <row r="617" spans="1:17">
       <c r="A617" s="3" t="s">
         <v>17</v>
       </c>
@@ -36292,7 +36330,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="618" spans="1:17" hidden="1">
+    <row r="618" spans="1:17">
       <c r="A618" s="3" t="s">
         <v>17</v>
       </c>
@@ -36343,7 +36381,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="619" spans="1:17" hidden="1">
+    <row r="619" spans="1:17">
       <c r="A619" s="3" t="s">
         <v>17</v>
       </c>
@@ -36394,7 +36432,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="620" spans="1:17" hidden="1">
+    <row r="620" spans="1:17">
       <c r="A620" s="3" t="s">
         <v>17</v>
       </c>
@@ -36445,7 +36483,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="621" spans="1:17" hidden="1">
+    <row r="621" spans="1:17">
       <c r="A621" s="3" t="s">
         <v>17</v>
       </c>
@@ -36496,7 +36534,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="622" spans="1:17" hidden="1">
+    <row r="622" spans="1:17">
       <c r="A622" s="3" t="s">
         <v>17</v>
       </c>
@@ -36547,7 +36585,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="623" spans="1:17" hidden="1">
+    <row r="623" spans="1:17">
       <c r="A623" s="3" t="s">
         <v>17</v>
       </c>
@@ -36598,7 +36636,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="624" spans="1:17" hidden="1">
+    <row r="624" spans="1:17">
       <c r="A624" s="3" t="s">
         <v>17</v>
       </c>
@@ -36649,7 +36687,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="625" spans="1:17" hidden="1">
+    <row r="625" spans="1:17">
       <c r="A625" s="3" t="s">
         <v>17</v>
       </c>
@@ -36700,7 +36738,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="626" spans="1:17" hidden="1">
+    <row r="626" spans="1:17">
       <c r="A626" s="3" t="s">
         <v>17</v>
       </c>
@@ -36751,7 +36789,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="627" spans="1:17" hidden="1">
+    <row r="627" spans="1:17">
       <c r="A627" s="3" t="s">
         <v>17</v>
       </c>
@@ -36802,7 +36840,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="628" spans="1:17" hidden="1">
+    <row r="628" spans="1:17">
       <c r="A628" s="3" t="s">
         <v>17</v>
       </c>
@@ -36853,7 +36891,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="629" spans="1:17" hidden="1">
+    <row r="629" spans="1:17">
       <c r="A629" s="3" t="s">
         <v>17</v>
       </c>
@@ -36904,7 +36942,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="630" spans="1:17" hidden="1">
+    <row r="630" spans="1:17">
       <c r="A630" s="3" t="s">
         <v>17</v>
       </c>
@@ -36955,7 +36993,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="631" spans="1:17" hidden="1">
+    <row r="631" spans="1:17">
       <c r="A631" s="3" t="s">
         <v>17</v>
       </c>
@@ -37006,7 +37044,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="632" spans="1:17" hidden="1">
+    <row r="632" spans="1:17">
       <c r="A632" s="3" t="s">
         <v>17</v>
       </c>
@@ -37057,7 +37095,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="633" spans="1:17" hidden="1">
+    <row r="633" spans="1:17">
       <c r="A633" s="3" t="s">
         <v>17</v>
       </c>
@@ -37108,7 +37146,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="634" spans="1:17" hidden="1">
+    <row r="634" spans="1:17">
       <c r="A634" s="3" t="s">
         <v>17</v>
       </c>
@@ -37159,7 +37197,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="635" spans="1:17" hidden="1">
+    <row r="635" spans="1:17">
       <c r="A635" s="3" t="s">
         <v>17</v>
       </c>
@@ -37210,7 +37248,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="636" spans="1:17" hidden="1">
+    <row r="636" spans="1:17">
       <c r="A636" s="3" t="s">
         <v>17</v>
       </c>
@@ -37261,7 +37299,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="637" spans="1:17" hidden="1">
+    <row r="637" spans="1:17">
       <c r="A637" s="3" t="s">
         <v>17</v>
       </c>
@@ -37312,7 +37350,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="638" spans="1:17" hidden="1">
+    <row r="638" spans="1:17">
       <c r="A638" s="3" t="s">
         <v>17</v>
       </c>
@@ -37363,7 +37401,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="639" spans="1:17" hidden="1">
+    <row r="639" spans="1:17">
       <c r="A639" s="3" t="s">
         <v>17</v>
       </c>
@@ -37414,7 +37452,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="640" spans="1:17" hidden="1">
+    <row r="640" spans="1:17">
       <c r="A640" s="3" t="s">
         <v>17</v>
       </c>
@@ -37465,7 +37503,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="641" spans="1:17" hidden="1">
+    <row r="641" spans="1:17">
       <c r="A641" s="3" t="s">
         <v>17</v>
       </c>
@@ -37516,7 +37554,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="642" spans="1:17" hidden="1">
+    <row r="642" spans="1:17">
       <c r="A642" s="3" t="s">
         <v>17</v>
       </c>
@@ -37567,7 +37605,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="643" spans="1:17" hidden="1">
+    <row r="643" spans="1:17">
       <c r="A643" s="3" t="s">
         <v>17</v>
       </c>
@@ -37618,7 +37656,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="644" spans="1:17" hidden="1">
+    <row r="644" spans="1:17">
       <c r="A644" s="3" t="s">
         <v>17</v>
       </c>
@@ -37669,7 +37707,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="645" spans="1:17" hidden="1">
+    <row r="645" spans="1:17">
       <c r="A645" s="3" t="s">
         <v>17</v>
       </c>
@@ -37720,7 +37758,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="646" spans="1:17" hidden="1">
+    <row r="646" spans="1:17">
       <c r="A646" s="3" t="s">
         <v>17</v>
       </c>
@@ -37771,7 +37809,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="647" spans="1:17" hidden="1">
+    <row r="647" spans="1:17">
       <c r="A647" s="3" t="s">
         <v>17</v>
       </c>
@@ -37822,7 +37860,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="648" spans="1:17" hidden="1">
+    <row r="648" spans="1:17">
       <c r="A648" s="3" t="s">
         <v>17</v>
       </c>
@@ -37873,7 +37911,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="649" spans="1:17" hidden="1">
+    <row r="649" spans="1:17">
       <c r="A649" s="3" t="s">
         <v>17</v>
       </c>
@@ -37924,7 +37962,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="650" spans="1:17" hidden="1">
+    <row r="650" spans="1:17">
       <c r="A650" s="3" t="s">
         <v>17</v>
       </c>
@@ -37975,7 +38013,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="651" spans="1:17" hidden="1">
+    <row r="651" spans="1:17">
       <c r="A651" s="3" t="s">
         <v>17</v>
       </c>
@@ -38026,7 +38064,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="652" spans="1:17" hidden="1">
+    <row r="652" spans="1:17">
       <c r="A652" s="3" t="s">
         <v>17</v>
       </c>
@@ -38077,7 +38115,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="653" spans="1:17" hidden="1">
+    <row r="653" spans="1:17">
       <c r="A653" s="3" t="s">
         <v>17</v>
       </c>
@@ -38128,7 +38166,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="654" spans="1:17" hidden="1">
+    <row r="654" spans="1:17">
       <c r="A654" s="3" t="s">
         <v>17</v>
       </c>
@@ -38179,7 +38217,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="655" spans="1:17" hidden="1">
+    <row r="655" spans="1:17">
       <c r="A655" s="3" t="s">
         <v>17</v>
       </c>
@@ -38230,7 +38268,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="656" spans="1:17" hidden="1">
+    <row r="656" spans="1:17">
       <c r="A656" s="3" t="s">
         <v>17</v>
       </c>
@@ -38281,7 +38319,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="657" spans="1:17" hidden="1">
+    <row r="657" spans="1:17">
       <c r="A657" s="3" t="s">
         <v>17</v>
       </c>
@@ -38332,7 +38370,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="658" spans="1:17" hidden="1">
+    <row r="658" spans="1:17">
       <c r="A658" s="3" t="s">
         <v>17</v>
       </c>
@@ -38383,7 +38421,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="659" spans="1:17" hidden="1">
+    <row r="659" spans="1:17">
       <c r="A659" s="3" t="s">
         <v>17</v>
       </c>
@@ -38434,7 +38472,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="660" spans="1:17" hidden="1">
+    <row r="660" spans="1:17">
       <c r="A660" s="3" t="s">
         <v>17</v>
       </c>
@@ -38485,7 +38523,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="661" spans="1:17" hidden="1">
+    <row r="661" spans="1:17">
       <c r="A661" s="3" t="s">
         <v>17</v>
       </c>
@@ -38536,7 +38574,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="662" spans="1:17" hidden="1">
+    <row r="662" spans="1:17">
       <c r="A662" s="3" t="s">
         <v>17</v>
       </c>
@@ -38587,7 +38625,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="663" spans="1:17" hidden="1">
+    <row r="663" spans="1:17">
       <c r="A663" s="3" t="s">
         <v>17</v>
       </c>
@@ -38638,7 +38676,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="664" spans="1:17" hidden="1">
+    <row r="664" spans="1:17">
       <c r="A664" s="3" t="s">
         <v>17</v>
       </c>
@@ -38689,7 +38727,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="665" spans="1:17" hidden="1">
+    <row r="665" spans="1:17">
       <c r="A665" s="3" t="s">
         <v>17</v>
       </c>
@@ -38740,7 +38778,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="666" spans="1:17" hidden="1">
+    <row r="666" spans="1:17">
       <c r="A666" s="3" t="s">
         <v>17</v>
       </c>
@@ -38791,7 +38829,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="667" spans="1:17" hidden="1">
+    <row r="667" spans="1:17">
       <c r="A667" s="3" t="s">
         <v>17</v>
       </c>
@@ -38842,7 +38880,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="668" spans="1:17" hidden="1">
+    <row r="668" spans="1:17">
       <c r="A668" s="3" t="s">
         <v>17</v>
       </c>
@@ -38893,7 +38931,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="669" spans="1:17" hidden="1">
+    <row r="669" spans="1:17">
       <c r="A669" s="3" t="s">
         <v>17</v>
       </c>
@@ -38944,7 +38982,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="670" spans="1:17" hidden="1">
+    <row r="670" spans="1:17">
       <c r="A670" s="3" t="s">
         <v>17</v>
       </c>
@@ -38995,7 +39033,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="671" spans="1:17" hidden="1">
+    <row r="671" spans="1:17">
       <c r="A671" s="3" t="s">
         <v>17</v>
       </c>
@@ -39046,7 +39084,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="672" spans="1:17" hidden="1">
+    <row r="672" spans="1:17">
       <c r="A672" s="3" t="s">
         <v>17</v>
       </c>
@@ -39097,7 +39135,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="673" spans="1:17" hidden="1">
+    <row r="673" spans="1:17">
       <c r="A673" s="3" t="s">
         <v>17</v>
       </c>
@@ -39148,7 +39186,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="674" spans="1:17" hidden="1">
+    <row r="674" spans="1:17">
       <c r="A674" s="3" t="s">
         <v>17</v>
       </c>
@@ -39199,7 +39237,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="675" spans="1:17" hidden="1">
+    <row r="675" spans="1:17">
       <c r="A675" s="3" t="s">
         <v>17</v>
       </c>
@@ -39250,7 +39288,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="676" spans="1:17" hidden="1">
+    <row r="676" spans="1:17">
       <c r="A676" s="3" t="s">
         <v>17</v>
       </c>
@@ -39301,7 +39339,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="677" spans="1:17" hidden="1">
+    <row r="677" spans="1:17">
       <c r="A677" s="3" t="s">
         <v>17</v>
       </c>
@@ -39352,7 +39390,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="678" spans="1:17" hidden="1">
+    <row r="678" spans="1:17">
       <c r="A678" s="3" t="s">
         <v>17</v>
       </c>
@@ -39403,7 +39441,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="679" spans="1:17" hidden="1">
+    <row r="679" spans="1:17">
       <c r="A679" s="3" t="s">
         <v>17</v>
       </c>
@@ -39454,7 +39492,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="680" spans="1:17" hidden="1">
+    <row r="680" spans="1:17">
       <c r="A680" s="3" t="s">
         <v>17</v>
       </c>
@@ -39505,7 +39543,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="681" spans="1:17" hidden="1">
+    <row r="681" spans="1:17">
       <c r="A681" s="3" t="s">
         <v>17</v>
       </c>
@@ -39556,7 +39594,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="682" spans="1:17" hidden="1">
+    <row r="682" spans="1:17">
       <c r="A682" s="3" t="s">
         <v>17</v>
       </c>
@@ -39607,7 +39645,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="683" spans="1:17" hidden="1">
+    <row r="683" spans="1:17">
       <c r="A683" s="3" t="s">
         <v>17</v>
       </c>
@@ -39658,7 +39696,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="684" spans="1:17" hidden="1">
+    <row r="684" spans="1:17">
       <c r="A684" s="3" t="s">
         <v>17</v>
       </c>
@@ -39709,7 +39747,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="685" spans="1:17" hidden="1">
+    <row r="685" spans="1:17">
       <c r="A685" s="3" t="s">
         <v>17</v>
       </c>
@@ -39760,7 +39798,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="686" spans="1:17" hidden="1">
+    <row r="686" spans="1:17">
       <c r="A686" s="3" t="s">
         <v>17</v>
       </c>
@@ -39811,7 +39849,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="687" spans="1:17" hidden="1">
+    <row r="687" spans="1:17">
       <c r="A687" s="3" t="s">
         <v>17</v>
       </c>
@@ -39862,7 +39900,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="688" spans="1:17" hidden="1">
+    <row r="688" spans="1:17">
       <c r="A688" s="3" t="s">
         <v>17</v>
       </c>
@@ -39913,7 +39951,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="689" spans="1:17" hidden="1">
+    <row r="689" spans="1:17">
       <c r="A689" s="3" t="s">
         <v>17</v>
       </c>
@@ -39964,7 +40002,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="690" spans="1:17" hidden="1">
+    <row r="690" spans="1:17">
       <c r="A690" s="3" t="s">
         <v>17</v>
       </c>
@@ -40015,7 +40053,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="691" spans="1:17" hidden="1">
+    <row r="691" spans="1:17">
       <c r="A691" s="3" t="s">
         <v>17</v>
       </c>
@@ -40066,7 +40104,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="692" spans="1:17" hidden="1">
+    <row r="692" spans="1:17">
       <c r="A692" s="3" t="s">
         <v>17</v>
       </c>
@@ -40117,7 +40155,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="693" spans="1:17" hidden="1">
+    <row r="693" spans="1:17">
       <c r="A693" s="3" t="s">
         <v>17</v>
       </c>
@@ -40168,7 +40206,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="694" spans="1:17" hidden="1">
+    <row r="694" spans="1:17">
       <c r="A694" s="3" t="s">
         <v>17</v>
       </c>
@@ -40219,7 +40257,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="695" spans="1:17" hidden="1">
+    <row r="695" spans="1:17">
       <c r="A695" s="3" t="s">
         <v>17</v>
       </c>
@@ -40270,7 +40308,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="696" spans="1:17" hidden="1">
+    <row r="696" spans="1:17">
       <c r="A696" s="3" t="s">
         <v>17</v>
       </c>
@@ -40321,7 +40359,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="697" spans="1:17" hidden="1">
+    <row r="697" spans="1:17">
       <c r="A697" s="3" t="s">
         <v>17</v>
       </c>
@@ -40372,7 +40410,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="698" spans="1:17" hidden="1">
+    <row r="698" spans="1:17">
       <c r="A698" s="3" t="s">
         <v>17</v>
       </c>
@@ -40423,7 +40461,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="699" spans="1:17" hidden="1">
+    <row r="699" spans="1:17">
       <c r="A699" s="3" t="s">
         <v>17</v>
       </c>
@@ -40474,7 +40512,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="700" spans="1:17" hidden="1">
+    <row r="700" spans="1:17">
       <c r="A700" s="3" t="s">
         <v>17</v>
       </c>
@@ -40525,7 +40563,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="701" spans="1:17" hidden="1">
+    <row r="701" spans="1:17">
       <c r="A701" s="3" t="s">
         <v>17</v>
       </c>
@@ -40576,7 +40614,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="702" spans="1:17" hidden="1">
+    <row r="702" spans="1:17">
       <c r="A702" s="3" t="s">
         <v>17</v>
       </c>
@@ -40627,7 +40665,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="703" spans="1:17" hidden="1">
+    <row r="703" spans="1:17">
       <c r="A703" s="3" t="s">
         <v>17</v>
       </c>
@@ -40678,7 +40716,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="704" spans="1:17" hidden="1">
+    <row r="704" spans="1:17">
       <c r="A704" s="3" t="s">
         <v>17</v>
       </c>
@@ -40729,7 +40767,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="705" spans="1:17" hidden="1">
+    <row r="705" spans="1:17">
       <c r="A705" s="3" t="s">
         <v>17</v>
       </c>
@@ -40780,7 +40818,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="706" spans="1:17" hidden="1">
+    <row r="706" spans="1:17">
       <c r="A706" s="3" t="s">
         <v>17</v>
       </c>
@@ -40831,7 +40869,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="707" spans="1:17" hidden="1">
+    <row r="707" spans="1:17">
       <c r="A707" s="3" t="s">
         <v>17</v>
       </c>
@@ -40882,7 +40920,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="708" spans="1:17" hidden="1">
+    <row r="708" spans="1:17">
       <c r="A708" s="3" t="s">
         <v>17</v>
       </c>
@@ -40933,7 +40971,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="709" spans="1:17" hidden="1">
+    <row r="709" spans="1:17">
       <c r="A709" s="3" t="s">
         <v>17</v>
       </c>
@@ -40984,7 +41022,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="710" spans="1:17" hidden="1">
+    <row r="710" spans="1:17">
       <c r="A710" s="3" t="s">
         <v>17</v>
       </c>
@@ -41035,7 +41073,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="711" spans="1:17" hidden="1">
+    <row r="711" spans="1:17">
       <c r="A711" s="3" t="s">
         <v>17</v>
       </c>
@@ -41086,7 +41124,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="712" spans="1:17" hidden="1">
+    <row r="712" spans="1:17">
       <c r="A712" s="3" t="s">
         <v>17</v>
       </c>
@@ -41137,7 +41175,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="713" spans="1:17" hidden="1">
+    <row r="713" spans="1:17">
       <c r="A713" s="3" t="s">
         <v>17</v>
       </c>
@@ -41188,7 +41226,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="714" spans="1:17" hidden="1">
+    <row r="714" spans="1:17">
       <c r="A714" s="3" t="s">
         <v>17</v>
       </c>
@@ -41239,7 +41277,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="715" spans="1:17" hidden="1">
+    <row r="715" spans="1:17">
       <c r="A715" s="3" t="s">
         <v>17</v>
       </c>
@@ -41290,7 +41328,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="716" spans="1:17" hidden="1">
+    <row r="716" spans="1:17">
       <c r="A716" s="3" t="s">
         <v>17</v>
       </c>
@@ -41341,7 +41379,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="717" spans="1:17" hidden="1">
+    <row r="717" spans="1:17">
       <c r="A717" s="3" t="s">
         <v>17</v>
       </c>
@@ -41392,7 +41430,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="718" spans="1:17" hidden="1">
+    <row r="718" spans="1:17">
       <c r="A718" s="3" t="s">
         <v>17</v>
       </c>
@@ -41443,7 +41481,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="719" spans="1:17" hidden="1">
+    <row r="719" spans="1:17">
       <c r="A719" s="3" t="s">
         <v>17</v>
       </c>
@@ -41494,7 +41532,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="720" spans="1:17" hidden="1">
+    <row r="720" spans="1:17">
       <c r="A720" s="3" t="s">
         <v>17</v>
       </c>
@@ -41545,7 +41583,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="721" spans="1:17" hidden="1">
+    <row r="721" spans="1:17">
       <c r="A721" s="3" t="s">
         <v>17</v>
       </c>
@@ -41596,7 +41634,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="722" spans="1:17" hidden="1">
+    <row r="722" spans="1:17">
       <c r="A722" s="3" t="s">
         <v>17</v>
       </c>
@@ -41647,7 +41685,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="723" spans="1:17" hidden="1">
+    <row r="723" spans="1:17">
       <c r="A723" s="3" t="s">
         <v>17</v>
       </c>
@@ -41698,7 +41736,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="724" spans="1:17" hidden="1">
+    <row r="724" spans="1:17">
       <c r="A724" s="3" t="s">
         <v>17</v>
       </c>
@@ -41749,7 +41787,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="725" spans="1:17" hidden="1">
+    <row r="725" spans="1:17">
       <c r="A725" s="3" t="s">
         <v>17</v>
       </c>
@@ -41800,7 +41838,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="726" spans="1:17" hidden="1">
+    <row r="726" spans="1:17">
       <c r="A726" s="3" t="s">
         <v>17</v>
       </c>
@@ -41851,7 +41889,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="727" spans="1:17" hidden="1">
+    <row r="727" spans="1:17">
       <c r="A727" s="3" t="s">
         <v>17</v>
       </c>
@@ -41902,7 +41940,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="728" spans="1:17" hidden="1">
+    <row r="728" spans="1:17">
       <c r="A728" s="3" t="s">
         <v>17</v>
       </c>
@@ -41953,7 +41991,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="729" spans="1:17" hidden="1">
+    <row r="729" spans="1:17">
       <c r="A729" s="3" t="s">
         <v>17</v>
       </c>
@@ -42004,7 +42042,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="730" spans="1:17" hidden="1">
+    <row r="730" spans="1:17">
       <c r="A730" s="3" t="s">
         <v>17</v>
       </c>
@@ -42055,7 +42093,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="731" spans="1:17" hidden="1">
+    <row r="731" spans="1:17">
       <c r="A731" s="3" t="s">
         <v>17</v>
       </c>
@@ -42106,7 +42144,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="732" spans="1:17" hidden="1">
+    <row r="732" spans="1:17">
       <c r="A732" s="3" t="s">
         <v>17</v>
       </c>
@@ -42157,7 +42195,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="733" spans="1:17" hidden="1">
+    <row r="733" spans="1:17">
       <c r="A733" s="3" t="s">
         <v>17</v>
       </c>
@@ -42208,7 +42246,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="734" spans="1:17" hidden="1">
+    <row r="734" spans="1:17">
       <c r="A734" s="3" t="s">
         <v>17</v>
       </c>
@@ -42259,7 +42297,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="735" spans="1:17" hidden="1">
+    <row r="735" spans="1:17">
       <c r="A735" s="3" t="s">
         <v>17</v>
       </c>
@@ -42310,7 +42348,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="736" spans="1:17" hidden="1">
+    <row r="736" spans="1:17">
       <c r="A736" s="3" t="s">
         <v>17</v>
       </c>
@@ -42361,7 +42399,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="737" spans="1:17" hidden="1">
+    <row r="737" spans="1:17">
       <c r="A737" s="3" t="s">
         <v>17</v>
       </c>
@@ -42412,7 +42450,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="738" spans="1:17" hidden="1">
+    <row r="738" spans="1:17">
       <c r="A738" s="3" t="s">
         <v>17</v>
       </c>
@@ -42463,7 +42501,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="739" spans="1:17" hidden="1">
+    <row r="739" spans="1:17">
       <c r="A739" s="3" t="s">
         <v>17</v>
       </c>
@@ -42514,7 +42552,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="740" spans="1:17" hidden="1">
+    <row r="740" spans="1:17">
       <c r="A740" s="3" t="s">
         <v>17</v>
       </c>
@@ -42565,7 +42603,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="741" spans="1:17" hidden="1">
+    <row r="741" spans="1:17">
       <c r="A741" s="3" t="s">
         <v>17</v>
       </c>
@@ -42616,7 +42654,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="742" spans="1:17" hidden="1">
+    <row r="742" spans="1:17">
       <c r="A742" s="3" t="s">
         <v>17</v>
       </c>
@@ -42667,7 +42705,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="743" spans="1:17" hidden="1">
+    <row r="743" spans="1:17">
       <c r="A743" s="3" t="s">
         <v>17</v>
       </c>
@@ -42718,7 +42756,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="744" spans="1:17" hidden="1">
+    <row r="744" spans="1:17">
       <c r="A744" s="3" t="s">
         <v>17</v>
       </c>
@@ -42769,7 +42807,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="745" spans="1:17" hidden="1">
+    <row r="745" spans="1:17">
       <c r="A745" s="3" t="s">
         <v>17</v>
       </c>
@@ -42820,7 +42858,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="746" spans="1:17" hidden="1">
+    <row r="746" spans="1:17">
       <c r="A746" s="3" t="s">
         <v>17</v>
       </c>
@@ -42871,7 +42909,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="747" spans="1:17" hidden="1">
+    <row r="747" spans="1:17">
       <c r="A747" s="3" t="s">
         <v>17</v>
       </c>
@@ -42922,7 +42960,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="748" spans="1:17" hidden="1">
+    <row r="748" spans="1:17">
       <c r="A748" s="3" t="s">
         <v>17</v>
       </c>
@@ -42973,7 +43011,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="749" spans="1:17" hidden="1">
+    <row r="749" spans="1:17">
       <c r="A749" s="3" t="s">
         <v>17</v>
       </c>
@@ -43024,7 +43062,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="750" spans="1:17" hidden="1">
+    <row r="750" spans="1:17">
       <c r="A750" s="3" t="s">
         <v>17</v>
       </c>
@@ -43075,7 +43113,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="751" spans="1:17" hidden="1">
+    <row r="751" spans="1:17">
       <c r="A751" s="3" t="s">
         <v>17</v>
       </c>
@@ -43126,7 +43164,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="752" spans="1:17" hidden="1">
+    <row r="752" spans="1:17">
       <c r="A752" s="3" t="s">
         <v>17</v>
       </c>
@@ -43177,7 +43215,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="753" spans="1:17" hidden="1">
+    <row r="753" spans="1:17">
       <c r="A753" s="3" t="s">
         <v>17</v>
       </c>
@@ -43228,7 +43266,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="754" spans="1:17" hidden="1">
+    <row r="754" spans="1:17">
       <c r="A754" s="3" t="s">
         <v>17</v>
       </c>
@@ -43279,7 +43317,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="755" spans="1:17" hidden="1">
+    <row r="755" spans="1:17">
       <c r="A755" s="3" t="s">
         <v>17</v>
       </c>
@@ -43330,7 +43368,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="756" spans="1:17" hidden="1">
+    <row r="756" spans="1:17">
       <c r="A756" s="3" t="s">
         <v>17</v>
       </c>
@@ -43381,7 +43419,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="757" spans="1:17" hidden="1">
+    <row r="757" spans="1:17">
       <c r="A757" s="3" t="s">
         <v>17</v>
       </c>
@@ -43432,7 +43470,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="758" spans="1:17" hidden="1">
+    <row r="758" spans="1:17">
       <c r="A758" s="3" t="s">
         <v>17</v>
       </c>
@@ -43483,7 +43521,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="759" spans="1:17" hidden="1">
+    <row r="759" spans="1:17">
       <c r="A759" s="3" t="s">
         <v>17</v>
       </c>
@@ -43534,7 +43572,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="760" spans="1:17" hidden="1">
+    <row r="760" spans="1:17">
       <c r="A760" s="3" t="s">
         <v>17</v>
       </c>
@@ -43585,7 +43623,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="761" spans="1:17" hidden="1">
+    <row r="761" spans="1:17">
       <c r="A761" s="3" t="s">
         <v>17</v>
       </c>
@@ -43636,7 +43674,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="762" spans="1:17" hidden="1">
+    <row r="762" spans="1:17">
       <c r="A762" s="3" t="s">
         <v>17</v>
       </c>
@@ -43687,7 +43725,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="763" spans="1:17" hidden="1">
+    <row r="763" spans="1:17">
       <c r="A763" s="3" t="s">
         <v>17</v>
       </c>
@@ -43738,7 +43776,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="764" spans="1:17" hidden="1">
+    <row r="764" spans="1:17">
       <c r="A764" s="3" t="s">
         <v>17</v>
       </c>
@@ -43789,7 +43827,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="765" spans="1:17" hidden="1">
+    <row r="765" spans="1:17">
       <c r="A765" s="3" t="s">
         <v>17</v>
       </c>
@@ -43840,7 +43878,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="766" spans="1:17" hidden="1">
+    <row r="766" spans="1:17">
       <c r="A766" s="3" t="s">
         <v>17</v>
       </c>
@@ -43891,7 +43929,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="767" spans="1:17" hidden="1">
+    <row r="767" spans="1:17">
       <c r="A767" s="3" t="s">
         <v>17</v>
       </c>
@@ -43942,7 +43980,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="768" spans="1:17" hidden="1">
+    <row r="768" spans="1:17">
       <c r="A768" s="3" t="s">
         <v>17</v>
       </c>
@@ -43993,7 +44031,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="769" spans="1:17" hidden="1">
+    <row r="769" spans="1:17">
       <c r="A769" s="3" t="s">
         <v>17</v>
       </c>
@@ -44044,7 +44082,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="770" spans="1:17" hidden="1">
+    <row r="770" spans="1:17">
       <c r="A770" s="3" t="s">
         <v>17</v>
       </c>
@@ -44095,7 +44133,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="771" spans="1:17" hidden="1">
+    <row r="771" spans="1:17">
       <c r="A771" s="3" t="s">
         <v>17</v>
       </c>
@@ -44146,7 +44184,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="772" spans="1:17" hidden="1">
+    <row r="772" spans="1:17">
       <c r="A772" s="3" t="s">
         <v>17</v>
       </c>
@@ -44197,7 +44235,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="773" spans="1:17" hidden="1">
+    <row r="773" spans="1:17">
       <c r="A773" s="3" t="s">
         <v>17</v>
       </c>
@@ -44248,7 +44286,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="774" spans="1:17" hidden="1">
+    <row r="774" spans="1:17">
       <c r="A774" s="3" t="s">
         <v>17</v>
       </c>
@@ -44299,7 +44337,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="775" spans="1:17" hidden="1">
+    <row r="775" spans="1:17">
       <c r="A775" s="3" t="s">
         <v>17</v>
       </c>
@@ -44350,7 +44388,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="776" spans="1:17" hidden="1">
+    <row r="776" spans="1:17">
       <c r="A776" s="3" t="s">
         <v>17</v>
       </c>
@@ -44401,7 +44439,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="777" spans="1:17" hidden="1">
+    <row r="777" spans="1:17">
       <c r="A777" s="3" t="s">
         <v>17</v>
       </c>
@@ -44452,7 +44490,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="778" spans="1:17" hidden="1">
+    <row r="778" spans="1:17">
       <c r="A778" s="3" t="s">
         <v>17</v>
       </c>
@@ -44503,7 +44541,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="779" spans="1:17" hidden="1">
+    <row r="779" spans="1:17">
       <c r="A779" s="3" t="s">
         <v>17</v>
       </c>
@@ -44554,7 +44592,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="780" spans="1:17" hidden="1">
+    <row r="780" spans="1:17">
       <c r="A780" s="3" t="s">
         <v>17</v>
       </c>
@@ -44605,7 +44643,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="781" spans="1:17" hidden="1">
+    <row r="781" spans="1:17">
       <c r="A781" s="3" t="s">
         <v>17</v>
       </c>
@@ -44656,7 +44694,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="782" spans="1:17" hidden="1">
+    <row r="782" spans="1:17">
       <c r="A782" s="3" t="s">
         <v>17</v>
       </c>
@@ -44707,7 +44745,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="783" spans="1:17" hidden="1">
+    <row r="783" spans="1:17">
       <c r="A783" s="3" t="s">
         <v>17</v>
       </c>
@@ -44758,7 +44796,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="784" spans="1:17" hidden="1">
+    <row r="784" spans="1:17">
       <c r="A784" s="3" t="s">
         <v>17</v>
       </c>
@@ -44809,7 +44847,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="785" spans="1:17" hidden="1">
+    <row r="785" spans="1:17">
       <c r="A785" s="3" t="s">
         <v>17</v>
       </c>
@@ -44860,7 +44898,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="786" spans="1:17" hidden="1">
+    <row r="786" spans="1:17">
       <c r="A786" s="3" t="s">
         <v>17</v>
       </c>
@@ -44911,7 +44949,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="787" spans="1:17" hidden="1">
+    <row r="787" spans="1:17">
       <c r="A787" s="3" t="s">
         <v>17</v>
       </c>
@@ -44962,7 +45000,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="788" spans="1:17" hidden="1">
+    <row r="788" spans="1:17">
       <c r="A788" s="3" t="s">
         <v>17</v>
       </c>
@@ -45013,7 +45051,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="789" spans="1:17" hidden="1">
+    <row r="789" spans="1:17">
       <c r="A789" s="3" t="s">
         <v>17</v>
       </c>
@@ -45064,7 +45102,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="790" spans="1:17" hidden="1">
+    <row r="790" spans="1:17">
       <c r="A790" s="3" t="s">
         <v>17</v>
       </c>
@@ -45115,7 +45153,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="791" spans="1:17" hidden="1">
+    <row r="791" spans="1:17">
       <c r="A791" s="3" t="s">
         <v>17</v>
       </c>
@@ -45166,7 +45204,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="792" spans="1:17" hidden="1">
+    <row r="792" spans="1:17">
       <c r="A792" s="3" t="s">
         <v>17</v>
       </c>
@@ -45217,7 +45255,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="793" spans="1:17" hidden="1">
+    <row r="793" spans="1:17">
       <c r="A793" s="3" t="s">
         <v>17</v>
       </c>
@@ -45268,7 +45306,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="794" spans="1:17" hidden="1">
+    <row r="794" spans="1:17">
       <c r="A794" s="3" t="s">
         <v>17</v>
       </c>
@@ -45319,7 +45357,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="795" spans="1:17" hidden="1">
+    <row r="795" spans="1:17">
       <c r="A795" s="3" t="s">
         <v>17</v>
       </c>
@@ -45370,7 +45408,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="796" spans="1:17" hidden="1">
+    <row r="796" spans="1:17">
       <c r="A796" s="3" t="s">
         <v>17</v>
       </c>
@@ -45421,7 +45459,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="797" spans="1:17" hidden="1">
+    <row r="797" spans="1:17">
       <c r="A797" s="3" t="s">
         <v>17</v>
       </c>
@@ -45472,7 +45510,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="798" spans="1:17" hidden="1">
+    <row r="798" spans="1:17">
       <c r="A798" s="3" t="s">
         <v>17</v>
       </c>
@@ -45523,7 +45561,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="799" spans="1:17" hidden="1">
+    <row r="799" spans="1:17">
       <c r="A799" s="3" t="s">
         <v>17</v>
       </c>
@@ -45574,7 +45612,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="800" spans="1:17" hidden="1">
+    <row r="800" spans="1:17">
       <c r="A800" s="3" t="s">
         <v>17</v>
       </c>
@@ -45625,7 +45663,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="801" spans="1:17" hidden="1">
+    <row r="801" spans="1:17">
       <c r="A801" s="3" t="s">
         <v>17</v>
       </c>
@@ -45676,7 +45714,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="802" spans="1:17" hidden="1">
+    <row r="802" spans="1:17">
       <c r="A802" s="3" t="s">
         <v>17</v>
       </c>
@@ -45727,7 +45765,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="803" spans="1:17" hidden="1">
+    <row r="803" spans="1:17">
       <c r="A803" s="3" t="s">
         <v>17</v>
       </c>
@@ -45778,7 +45816,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="804" spans="1:17" hidden="1">
+    <row r="804" spans="1:17">
       <c r="A804" s="3" t="s">
         <v>17</v>
       </c>
@@ -45829,7 +45867,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="805" spans="1:17" hidden="1">
+    <row r="805" spans="1:17">
       <c r="A805" s="3" t="s">
         <v>17</v>
       </c>
@@ -45880,7 +45918,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="806" spans="1:17" hidden="1">
+    <row r="806" spans="1:17">
       <c r="A806" s="3" t="s">
         <v>17</v>
       </c>
@@ -45931,7 +45969,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="807" spans="1:17" hidden="1">
+    <row r="807" spans="1:17">
       <c r="A807" s="3" t="s">
         <v>17</v>
       </c>
@@ -45982,7 +46020,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="808" spans="1:17" hidden="1">
+    <row r="808" spans="1:17">
       <c r="A808" s="3" t="s">
         <v>17</v>
       </c>
@@ -46033,7 +46071,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="809" spans="1:17" hidden="1">
+    <row r="809" spans="1:17">
       <c r="A809" s="3" t="s">
         <v>17</v>
       </c>
@@ -46084,7 +46122,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="810" spans="1:17" hidden="1">
+    <row r="810" spans="1:17">
       <c r="A810" s="3" t="s">
         <v>17</v>
       </c>
@@ -46135,7 +46173,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="811" spans="1:17" hidden="1">
+    <row r="811" spans="1:17">
       <c r="A811" s="3" t="s">
         <v>17</v>
       </c>
@@ -46186,7 +46224,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="812" spans="1:17" hidden="1">
+    <row r="812" spans="1:17">
       <c r="A812" s="3" t="s">
         <v>17</v>
       </c>
@@ -46237,7 +46275,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="813" spans="1:17" hidden="1">
+    <row r="813" spans="1:17">
       <c r="A813" s="3" t="s">
         <v>17</v>
       </c>
@@ -46288,7 +46326,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="814" spans="1:17" hidden="1">
+    <row r="814" spans="1:17">
       <c r="A814" s="3" t="s">
         <v>17</v>
       </c>
@@ -46339,7 +46377,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="815" spans="1:17" hidden="1">
+    <row r="815" spans="1:17">
       <c r="A815" s="3" t="s">
         <v>17</v>
       </c>
@@ -46390,7 +46428,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="816" spans="1:17" hidden="1">
+    <row r="816" spans="1:17">
       <c r="A816" s="3" t="s">
         <v>17</v>
       </c>
@@ -46441,7 +46479,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="817" spans="1:17" hidden="1">
+    <row r="817" spans="1:17">
       <c r="A817" s="3" t="s">
         <v>17</v>
       </c>
@@ -46492,7 +46530,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="818" spans="1:17" hidden="1">
+    <row r="818" spans="1:17">
       <c r="A818" s="3" t="s">
         <v>17</v>
       </c>
@@ -46543,7 +46581,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="819" spans="1:17" hidden="1">
+    <row r="819" spans="1:17">
       <c r="A819" s="3" t="s">
         <v>17</v>
       </c>
@@ -46594,7 +46632,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="820" spans="1:17" hidden="1">
+    <row r="820" spans="1:17">
       <c r="A820" s="3" t="s">
         <v>17</v>
       </c>
@@ -46645,7 +46683,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="821" spans="1:17" hidden="1">
+    <row r="821" spans="1:17">
       <c r="A821" s="3" t="s">
         <v>17</v>
       </c>
@@ -46696,7 +46734,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="822" spans="1:17" hidden="1">
+    <row r="822" spans="1:17">
       <c r="A822" s="3" t="s">
         <v>17</v>
       </c>
@@ -46747,7 +46785,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="823" spans="1:17" hidden="1">
+    <row r="823" spans="1:17">
       <c r="A823" s="3" t="s">
         <v>17</v>
       </c>
@@ -46798,7 +46836,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="824" spans="1:17" hidden="1">
+    <row r="824" spans="1:17">
       <c r="A824" s="3" t="s">
         <v>17</v>
       </c>
@@ -46849,7 +46887,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="825" spans="1:17" hidden="1">
+    <row r="825" spans="1:17">
       <c r="A825" s="3" t="s">
         <v>17</v>
       </c>
@@ -46900,7 +46938,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="826" spans="1:17" hidden="1">
+    <row r="826" spans="1:17">
       <c r="A826" s="3" t="s">
         <v>17</v>
       </c>
@@ -46951,7 +46989,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="827" spans="1:17" hidden="1">
+    <row r="827" spans="1:17">
       <c r="A827" s="3" t="s">
         <v>17</v>
       </c>
@@ -47002,7 +47040,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="828" spans="1:17" hidden="1">
+    <row r="828" spans="1:17">
       <c r="A828" s="3" t="s">
         <v>17</v>
       </c>
@@ -47053,7 +47091,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="829" spans="1:17" hidden="1">
+    <row r="829" spans="1:17">
       <c r="A829" s="3" t="s">
         <v>17</v>
       </c>
@@ -47104,7 +47142,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="830" spans="1:17" hidden="1">
+    <row r="830" spans="1:17">
       <c r="A830" s="3" t="s">
         <v>17</v>
       </c>
@@ -47155,7 +47193,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="831" spans="1:17" hidden="1">
+    <row r="831" spans="1:17">
       <c r="A831" s="3" t="s">
         <v>17</v>
       </c>
@@ -47206,7 +47244,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="832" spans="1:17" hidden="1">
+    <row r="832" spans="1:17">
       <c r="A832" s="3" t="s">
         <v>17</v>
       </c>
@@ -47257,7 +47295,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="833" spans="1:17" hidden="1">
+    <row r="833" spans="1:17">
       <c r="A833" s="3" t="s">
         <v>17</v>
       </c>
@@ -47308,7 +47346,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="834" spans="1:17" hidden="1">
+    <row r="834" spans="1:17">
       <c r="A834" s="3" t="s">
         <v>17</v>
       </c>
@@ -47359,7 +47397,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="835" spans="1:17" hidden="1">
+    <row r="835" spans="1:17">
       <c r="A835" s="3" t="s">
         <v>17</v>
       </c>
@@ -47410,7 +47448,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="836" spans="1:17" hidden="1">
+    <row r="836" spans="1:17">
       <c r="A836" s="3" t="s">
         <v>17</v>
       </c>
@@ -47461,7 +47499,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="837" spans="1:17" hidden="1">
+    <row r="837" spans="1:17">
       <c r="A837" s="3" t="s">
         <v>17</v>
       </c>
@@ -47512,7 +47550,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="838" spans="1:17" hidden="1">
+    <row r="838" spans="1:17">
       <c r="A838" s="3" t="s">
         <v>17</v>
       </c>
@@ -47563,7 +47601,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="839" spans="1:17" hidden="1">
+    <row r="839" spans="1:17">
       <c r="A839" s="3" t="s">
         <v>17</v>
       </c>
@@ -47614,7 +47652,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="840" spans="1:17" hidden="1">
+    <row r="840" spans="1:17">
       <c r="A840" s="3" t="s">
         <v>17</v>
       </c>
@@ -47665,7 +47703,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="841" spans="1:17" hidden="1">
+    <row r="841" spans="1:17">
       <c r="A841" s="3" t="s">
         <v>17</v>
       </c>
@@ -47716,7 +47754,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="842" spans="1:17" hidden="1">
+    <row r="842" spans="1:17">
       <c r="A842" s="3" t="s">
         <v>17</v>
       </c>
@@ -47767,7 +47805,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="843" spans="1:17" hidden="1">
+    <row r="843" spans="1:17">
       <c r="A843" s="3" t="s">
         <v>17</v>
       </c>
@@ -47818,7 +47856,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="844" spans="1:17" hidden="1">
+    <row r="844" spans="1:17">
       <c r="A844" s="3" t="s">
         <v>17</v>
       </c>
@@ -47869,7 +47907,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="845" spans="1:17" hidden="1">
+    <row r="845" spans="1:17">
       <c r="A845" s="3" t="s">
         <v>17</v>
       </c>
@@ -47920,7 +47958,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="846" spans="1:17" hidden="1">
+    <row r="846" spans="1:17">
       <c r="A846" s="3" t="s">
         <v>17</v>
       </c>
@@ -47971,7 +48009,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="847" spans="1:17" hidden="1">
+    <row r="847" spans="1:17">
       <c r="A847" s="3" t="s">
         <v>17</v>
       </c>
@@ -48022,7 +48060,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="848" spans="1:17" hidden="1">
+    <row r="848" spans="1:17">
       <c r="A848" s="3" t="s">
         <v>17</v>
       </c>
@@ -48073,7 +48111,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="849" spans="1:17" hidden="1">
+    <row r="849" spans="1:17">
       <c r="A849" s="3" t="s">
         <v>17</v>
       </c>
@@ -53744,24 +53782,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:Q955" xr:uid="{6FA735D7-2150-4F79-92A5-3A08A686DD11}">
-    <filterColumn colId="2">
+    <filterColumn colId="13">
       <filters>
-        <filter val="AUDBasis6m3m10Y"/>
-        <filter val="AUDBasis6m3m12Y"/>
-        <filter val="AUDBasis6m3m15Y"/>
-        <filter val="AUDBasis6m3m1Y"/>
-        <filter val="AUDBasis6m3m20Y"/>
-        <filter val="AUDBasis6m3m25Y"/>
-        <filter val="AUDBasis6m3m2Y"/>
-        <filter val="AUDBasis6m3m30Y"/>
-        <filter val="AUDBasis6m3m3Y"/>
-        <filter val="AUDBasis6m3m4Y"/>
-        <filter val="AUDBasis6m3m5Y"/>
-        <filter val="AUDBasis6m3m6M"/>
-        <filter val="AUDBasis6m3m6Y"/>
-        <filter val="AUDBasis6m3m7Y"/>
-        <filter val="AUDBasis6m3m8Y"/>
-        <filter val="AUDBasis6m3m9Y"/>
+        <filter val="Daily"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -53771,6 +53794,427 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F4AEC44-8458-42D5-A030-87ADA58A9D39}">
+  <dimension ref="A1:P8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>1070</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1061</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.03</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1062</v>
+      </c>
+      <c r="D3" s="3">
+        <v>4.5499999999999999E-2</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N3" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1063</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="M4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0.65600000000000003</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N5" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1065</v>
+      </c>
+      <c r="D6" s="3">
+        <v>7.5800000000000006E-2</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N6" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="O6" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="D7" s="3">
+        <v>0.09</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>1068</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N7" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="O7" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>1060</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1067</v>
+      </c>
+      <c r="D8" s="3">
+        <v>1.12E-2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>1069</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N8" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>578</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="14" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D15F016-545C-4799-8823-9BED9F0DFD9E}">
   <dimension ref="A1:N126"/>
   <sheetViews>
@@ -59329,11 +59773,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{048FC3F1-C0DA-4A82-8D82-D964458877AB}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>

</xml_diff>